<commit_message>
challengers and gc update
</commit_message>
<xml_diff>
--- a/Data/Mappings/role_dict.xlsx
+++ b/Data/Mappings/role_dict.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hoo Kai Sng\Documents\Projects\VCT Hackathon\VCT-Hackathon-\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hoo Kai Sng\Documents\Projects\VCT Hackathon\VCT-Hackathon-\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{851F75B1-5E9B-4D58-9D52-D0B26926860F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547D2A68-A1B9-4BC9-808E-DFFAE0480F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5B3505EC-D04C-4C24-90B0-0E4C8036F7DA}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>agent_name</t>
   </si>
@@ -28,33 +28,15 @@
     <t>agent_role</t>
   </si>
   <si>
-    <t>team_role_1</t>
-  </si>
-  <si>
-    <t>team_role_2</t>
-  </si>
-  <si>
-    <t>team_role_3</t>
-  </si>
-  <si>
     <t>Brimstone</t>
   </si>
   <si>
     <t>Controller</t>
   </si>
   <si>
-    <t>Smoker</t>
-  </si>
-  <si>
     <t>Viper</t>
   </si>
   <si>
-    <t>Lurker</t>
-  </si>
-  <si>
-    <t>Anchor</t>
-  </si>
-  <si>
     <t>Omen</t>
   </si>
   <si>
@@ -73,15 +55,9 @@
     <t>Duelist</t>
   </si>
   <si>
-    <t>Flex</t>
-  </si>
-  <si>
     <t>Phoenix</t>
   </si>
   <si>
-    <t>Entry</t>
-  </si>
-  <si>
     <t>Jett</t>
   </si>
   <si>
@@ -103,13 +79,7 @@
     <t>Initiator</t>
   </si>
   <si>
-    <t>Flash</t>
-  </si>
-  <si>
     <t>Fade</t>
-  </si>
-  <si>
-    <t>Recon</t>
   </si>
   <si>
     <t>Skye</t>
@@ -626,8 +596,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1003,347 +974,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1823470E-C365-4AC7-B98D-FA7031EBF113}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
       <c r="B26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1352,6 +1202,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006E100AE026926B49996AF0740E5EEEDC" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c852d227d2a5603b8bea3d5fc9121e5d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b55da9b1-eea5-4863-a1cb-d51bd77dfd29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8adc258113501a3774bd216ac09e2e5e" ns3:_="">
     <xsd:import namespace="b55da9b1-eea5-4863-a1cb-d51bd77dfd29"/>
@@ -1495,15 +1354,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1511,6 +1361,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D91ACC8-4E7A-43CA-8C40-1111B55BF184}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97DF8026-5387-47E9-BEC1-A1ED40DD9437}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1524,14 +1382,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D91ACC8-4E7A-43CA-8C40-1111B55BF184}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>